<commit_message>
[ ADD SUPPORT OF NO TOKEN OF DIAGNOSTIC SIGNALS AND DIAGNOSTIC FRAMES ]
</commit_message>
<xml_diff>
--- a/TEST_QUEUE/LINBasicISC.xlsx
+++ b/TEST_QUEUE/LINBasicISC.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="63">
   <si>
     <t>LIN protocol version</t>
   </si>
@@ -149,27 +149,15 @@
     <t>constant_Signal</t>
   </si>
   <si>
-    <t>constant_Signal_Sig_Type,
-physical, 0, 255, 1.0, 0.0, None</t>
-  </si>
-  <si>
     <t>LinMsg1</t>
   </si>
   <si>
     <t>Sine</t>
   </si>
   <si>
-    <t>Sine_Sig_Type,
-physical, 0, 255, 1.0, 0.0, None</t>
-  </si>
-  <si>
     <t>Ramp</t>
   </si>
   <si>
-    <t>StandardPhys_Sig_Type,
-physical, 0, 0, 1.0, 0.0, None</t>
-  </si>
-  <si>
     <t>LinMsg2</t>
   </si>
   <si>
@@ -186,60 +174,6 @@
   </si>
   <si>
     <t>InitValue</t>
-  </si>
-  <si>
-    <t>MasterReq</t>
-  </si>
-  <si>
-    <t>MasterReqB0</t>
-  </si>
-  <si>
-    <t>MasterReqB1</t>
-  </si>
-  <si>
-    <t>MasterReqB2</t>
-  </si>
-  <si>
-    <t>MasterReqB3</t>
-  </si>
-  <si>
-    <t>MasterReqB4</t>
-  </si>
-  <si>
-    <t>MasterReqB5</t>
-  </si>
-  <si>
-    <t>MasterReqB6</t>
-  </si>
-  <si>
-    <t>MasterReqB7</t>
-  </si>
-  <si>
-    <t>SlaveResp</t>
-  </si>
-  <si>
-    <t>SlaveRespB0</t>
-  </si>
-  <si>
-    <t>SlaveRespB1</t>
-  </si>
-  <si>
-    <t>SlaveRespB2</t>
-  </si>
-  <si>
-    <t>SlaveRespB3</t>
-  </si>
-  <si>
-    <t>SlaveRespB4</t>
-  </si>
-  <si>
-    <t>SlaveRespB5</t>
-  </si>
-  <si>
-    <t>SlaveRespB6</t>
-  </si>
-  <si>
-    <t>SlaveRespB7</t>
   </si>
   <si>
     <t>Type</t>
@@ -336,16 +270,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -942,13 +873,13 @@
       <c r="I2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>41</v>
+      <c r="J2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="60" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="2">
         <v>48</v>
@@ -957,7 +888,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="2">
         <v>0</v>
@@ -974,13 +905,13 @@
       <c r="I3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>44</v>
+      <c r="J3" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="60" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="2">
         <v>48</v>
@@ -989,7 +920,7 @@
         <v>2</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E4" s="2">
         <v>8</v>
@@ -1006,13 +937,13 @@
       <c r="I4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>46</v>
+      <c r="J4" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="60" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B5" s="2">
         <v>38</v>
@@ -1038,13 +969,13 @@
       <c r="I5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>41</v>
+      <c r="J5" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="60" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2">
         <v>39</v>
@@ -1082,7 +1013,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1099,336 +1030,16 @@
         <v>30</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="2">
-        <v>60</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="2">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2">
-        <v>8</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" s="2">
-        <v>60</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D3" s="2">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2">
-        <v>8</v>
-      </c>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="2">
-        <v>60</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D4" s="2">
-        <v>16</v>
-      </c>
-      <c r="E4" s="2">
-        <v>8</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="2">
-        <v>60</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="2">
-        <v>24</v>
-      </c>
-      <c r="E5" s="2">
-        <v>8</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="2">
-        <v>60</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="2">
-        <v>32</v>
-      </c>
-      <c r="E6" s="2">
-        <v>8</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="2">
-        <v>60</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="2">
-        <v>40</v>
-      </c>
-      <c r="E7" s="2">
-        <v>8</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="2">
-        <v>60</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D8" s="2">
-        <v>48</v>
-      </c>
-      <c r="E8" s="2">
-        <v>8</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="2">
-        <v>60</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="2">
-        <v>56</v>
-      </c>
-      <c r="E9" s="2">
-        <v>8</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B10" s="2">
-        <v>61</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0</v>
-      </c>
-      <c r="E10" s="2">
-        <v>8</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="2">
-        <v>61</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D11" s="2">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2">
-        <v>8</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="2">
-        <v>61</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="2">
-        <v>16</v>
-      </c>
-      <c r="E12" s="2">
-        <v>8</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="A13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="2">
-        <v>61</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="2">
-        <v>24</v>
-      </c>
-      <c r="E13" s="2">
-        <v>8</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="2">
-        <v>61</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="2">
-        <v>32</v>
-      </c>
-      <c r="E14" s="2">
-        <v>8</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="2">
-        <v>61</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="2">
-        <v>40</v>
-      </c>
-      <c r="E15" s="2">
-        <v>8</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="2">
-        <v>61</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="2">
-        <v>48</v>
-      </c>
-      <c r="E16" s="2">
-        <v>8</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
-      <c r="A17" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="2">
-        <v>61</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D17" s="2">
-        <v>56</v>
-      </c>
-      <c r="E17" s="2">
-        <v>8</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1452,19 +1063,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1489,36 +1100,36 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="2" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="D2" s="2">
         <v>30</v>
@@ -1534,54 +1145,54 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="B3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="B3" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="3">
         <v>30</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G3" s="4" t="s">
+      <c r="E3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7">
-      <c r="B4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="B4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="3">
         <v>30</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="4" t="s">
+      <c r="E4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="2" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="D5" s="2">
         <v>10</v>
@@ -1597,22 +1208,22 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="B6" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="B6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="3">
         <v>10</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="4" t="s">
+      <c r="E6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>